<commit_message>
working / tied-out files
</commit_message>
<xml_diff>
--- a/CR_AdjCostBasis2023.xlsx
+++ b/CR_AdjCostBasis2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\all_programming\R_files\Financial\Allocate_df\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFBE0350-9ED1-4A26-A85C-DE9B17DE900F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20FBB712-5F19-4470-B307-D7FE995D6EC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25560" yWindow="2175" windowWidth="15645" windowHeight="11355" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26280" yWindow="2190" windowWidth="15645" windowHeight="11355" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tradesdownload.csv" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="AI" sheetId="2" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">AMC_BuySell!$A$1:$F$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">AMC_BuySell!$A$1:$F$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">tradesdownload.csv!$A$1:$I$291</definedName>
     <definedName name="_p2">AMC_Analysis!$N$17</definedName>
     <definedName name="_p3">AMC_Analysis!$N$23</definedName>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1413" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1426" uniqueCount="68">
   <si>
     <t>Sell</t>
   </si>
@@ -289,10 +289,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0000"/>
-    <numFmt numFmtId="166" formatCode="0_);[Red]\(0\)"/>
-    <numFmt numFmtId="168" formatCode="0.00_);[Red]\(0.00\)"/>
+    <numFmt numFmtId="165" formatCode="0_);[Red]\(0\)"/>
+    <numFmt numFmtId="166" formatCode="0.00_);[Red]\(0.00\)"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -427,14 +427,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -614,6 +608,18 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39994506668294322"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59996337778862885"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -784,7 +790,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -798,10 +804,16 @@
     <xf numFmtId="2" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1198,10 +1210,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:H291"/>
+  <dimension ref="A1:K291"/>
   <sheetViews>
-    <sheetView topLeftCell="A219" workbookViewId="0">
-      <selection activeCell="F295" sqref="F295"/>
+    <sheetView topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="H221" sqref="H221"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3615,7 +3627,7 @@
         <v>39688.22</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>44984</v>
       </c>
@@ -3635,7 +3647,7 @@
         <v>20221.79</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>44984</v>
       </c>
@@ -3654,8 +3666,12 @@
       <c r="F162" s="2">
         <v>14031.86</v>
       </c>
-    </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K162">
+        <f>SUBTOTAL(9,F161:F163)</f>
+        <v>42069.43</v>
+      </c>
+    </row>
+    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>44984</v>
       </c>
@@ -3675,7 +3691,7 @@
         <v>7815.78</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>44988</v>
       </c>
@@ -3695,7 +3711,7 @@
         <v>19653.3</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>44993</v>
       </c>
@@ -3715,7 +3731,7 @@
         <v>2922.4</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>44993</v>
       </c>
@@ -3735,7 +3751,7 @@
         <v>17834.41</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>44993</v>
       </c>
@@ -3755,7 +3771,7 @@
         <v>11509.61</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>44993</v>
       </c>
@@ -3775,7 +3791,7 @@
         <v>2859.9</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>45022</v>
       </c>
@@ -3795,7 +3811,7 @@
         <v>9829.6299999999992</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>45036</v>
       </c>
@@ -3815,7 +3831,7 @@
         <v>14967.64</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>45036</v>
       </c>
@@ -3835,7 +3851,7 @@
         <v>944.26</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>45036</v>
       </c>
@@ -3855,7 +3871,7 @@
         <v>4954.8100000000004</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>45036</v>
       </c>
@@ -3875,7 +3891,7 @@
         <v>4005.29</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>45076</v>
       </c>
@@ -3895,7 +3911,7 @@
         <v>4582.6099999999997</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>45079</v>
       </c>
@@ -3914,8 +3930,16 @@
       <c r="F175" s="2">
         <v>4993.8</v>
       </c>
-    </row>
-    <row r="176" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H175" s="2">
+        <f>SUBTOTAL(9,F152:F175)</f>
+        <v>223016.36999999997</v>
+      </c>
+      <c r="I175">
+        <f>SUBTOTAL(9,D152:D175)</f>
+        <v>36950</v>
+      </c>
+    </row>
+    <row r="176" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" s="1"/>
     </row>
     <row r="177" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -5835,8 +5859,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2B93BAD-2A26-43A9-9CCE-7DD98B0A8555}">
   <dimension ref="A1:N257"/>
   <sheetViews>
-    <sheetView topLeftCell="A177" workbookViewId="0">
-      <selection activeCell="I187" sqref="I187"/>
+    <sheetView tabSelected="1" topLeftCell="A190" workbookViewId="0">
+      <selection activeCell="I207" sqref="I207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5844,7 +5868,9 @@
     <col min="1" max="1" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" customWidth="1"/>
     <col min="10" max="10" width="12" customWidth="1"/>
+    <col min="11" max="11" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -9078,7 +9104,7 @@
         <v>3680.01</v>
       </c>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>45020</v>
       </c>
@@ -9098,7 +9124,7 @@
         <v>4163.45</v>
       </c>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>45020</v>
       </c>
@@ -9118,7 +9144,7 @@
         <v>124.88</v>
       </c>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>45020</v>
       </c>
@@ -9138,7 +9164,7 @@
         <v>37336.03</v>
       </c>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>45022</v>
       </c>
@@ -9158,7 +9184,7 @@
         <v>42239.51</v>
       </c>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>45037</v>
       </c>
@@ -9178,7 +9204,7 @@
         <v>13759.04</v>
       </c>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>45037</v>
       </c>
@@ -9198,7 +9224,7 @@
         <v>3994.16</v>
       </c>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <v>45037</v>
       </c>
@@ -9218,7 +9244,7 @@
         <v>22132.400000000001</v>
       </c>
     </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <v>45041</v>
       </c>
@@ -9238,7 +9264,7 @@
         <v>21700.35</v>
       </c>
     </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>45257</v>
       </c>
@@ -9258,7 +9284,7 @@
         <v>7399.91</v>
       </c>
     </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <v>45258</v>
       </c>
@@ -9286,7 +9312,7 @@
         <v>156518.69</v>
       </c>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <v>44953</v>
       </c>
@@ -9305,8 +9331,16 @@
       <c r="F188" s="2">
         <v>5512.12</v>
       </c>
-    </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I188" s="2">
+        <f>F188</f>
+        <v>5512.12</v>
+      </c>
+      <c r="K188">
+        <f>D188</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
         <v>44960</v>
       </c>
@@ -9325,8 +9359,9 @@
       <c r="F189" s="2">
         <v>6011.82</v>
       </c>
-    </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I189" s="2"/>
+    </row>
+    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <v>44960</v>
       </c>
@@ -9345,8 +9380,16 @@
       <c r="F190" s="2">
         <v>668.47</v>
       </c>
-    </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I190" s="2">
+        <f>F189+F190</f>
+        <v>6680.29</v>
+      </c>
+      <c r="K190">
+        <f>D189+D190</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <v>44960</v>
       </c>
@@ -9365,8 +9408,16 @@
       <c r="F191" s="2">
         <v>6254.7</v>
       </c>
-    </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I191" s="2">
+        <f>F191</f>
+        <v>6254.7</v>
+      </c>
+      <c r="K191">
+        <f>D191</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <v>44960</v>
       </c>
@@ -9385,8 +9436,16 @@
       <c r="F192" s="2">
         <v>6189.8</v>
       </c>
-    </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I192" s="2">
+        <f>F192</f>
+        <v>6189.8</v>
+      </c>
+      <c r="K192">
+        <f>D192</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="193" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <v>44978</v>
       </c>
@@ -9405,8 +9464,16 @@
       <c r="F193" s="2">
         <v>17564.150000000001</v>
       </c>
-    </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I193" s="2">
+        <f>F193</f>
+        <v>17564.150000000001</v>
+      </c>
+      <c r="K193">
+        <f>D193</f>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="194" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <v>44979</v>
       </c>
@@ -9425,8 +9492,16 @@
       <c r="F194" s="2">
         <v>39688.22</v>
       </c>
-    </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I194" s="2">
+        <f>F194</f>
+        <v>39688.22</v>
+      </c>
+      <c r="K194">
+        <f>D194</f>
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="195" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
         <v>44984</v>
       </c>
@@ -9445,8 +9520,16 @@
       <c r="F195" s="2">
         <v>20221.79</v>
       </c>
-    </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I195" s="2">
+        <f>F195</f>
+        <v>20221.79</v>
+      </c>
+      <c r="K195">
+        <f>D195</f>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="196" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <v>44984</v>
       </c>
@@ -9465,8 +9548,14 @@
       <c r="F196" s="2">
         <v>14031.86</v>
       </c>
-    </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I196" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K196" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="197" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <v>44984</v>
       </c>
@@ -9485,8 +9574,16 @@
       <c r="F197" s="2">
         <v>7815.78</v>
       </c>
-    </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I197" s="2">
+        <f>F196+F197</f>
+        <v>21847.64</v>
+      </c>
+      <c r="K197">
+        <f>D196+D197</f>
+        <v>2850</v>
+      </c>
+    </row>
+    <row r="198" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <v>44988</v>
       </c>
@@ -9505,8 +9602,16 @@
       <c r="F198" s="2">
         <v>19653.3</v>
       </c>
-    </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I198" s="2">
+        <f>F198</f>
+        <v>19653.3</v>
+      </c>
+      <c r="K198">
+        <f>D198</f>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="199" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
         <v>44993</v>
       </c>
@@ -9525,8 +9630,9 @@
       <c r="F199" s="2">
         <v>2922.4</v>
       </c>
-    </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I199" s="2"/>
+    </row>
+    <row r="200" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <v>44993</v>
       </c>
@@ -9545,8 +9651,12 @@
       <c r="F200" s="2">
         <v>17834.41</v>
       </c>
-    </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I200" s="2"/>
+      <c r="K200" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="201" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>44993</v>
       </c>
@@ -9565,8 +9675,9 @@
       <c r="F201" s="2">
         <v>11509.61</v>
       </c>
-    </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I201" s="2"/>
+    </row>
+    <row r="202" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
         <v>44993</v>
       </c>
@@ -9585,8 +9696,16 @@
       <c r="F202" s="2">
         <v>2859.9</v>
       </c>
-    </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I202" s="2">
+        <f>F199+F200+F201+F202</f>
+        <v>35126.32</v>
+      </c>
+      <c r="K202">
+        <f>D202+D201+D200+D199</f>
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="203" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
         <v>45022</v>
       </c>
@@ -9605,8 +9724,16 @@
       <c r="F203" s="2">
         <v>9829.6299999999992</v>
       </c>
-    </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I203" s="2">
+        <f>F203</f>
+        <v>9829.6299999999992</v>
+      </c>
+      <c r="K203">
+        <f>D203</f>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="204" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
         <v>45036</v>
       </c>
@@ -9625,8 +9752,9 @@
       <c r="F204" s="2">
         <v>14967.64</v>
       </c>
-    </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I204" s="2"/>
+    </row>
+    <row r="205" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
         <v>45036</v>
       </c>
@@ -9645,8 +9773,9 @@
       <c r="F205" s="2">
         <v>944.26</v>
       </c>
-    </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I205" s="2"/>
+    </row>
+    <row r="206" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
         <v>45036</v>
       </c>
@@ -9665,8 +9794,16 @@
       <c r="F206" s="2">
         <v>4954.8100000000004</v>
       </c>
-    </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I206" s="2">
+        <f>F204+F205+F206+F207</f>
+        <v>24872</v>
+      </c>
+      <c r="K206">
+        <f>D207+D206+D205+D204</f>
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="207" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
         <v>45036</v>
       </c>
@@ -9685,8 +9822,16 @@
       <c r="F207" s="2">
         <v>4005.29</v>
       </c>
-    </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I207" s="2">
+        <f>F208</f>
+        <v>4582.6099999999997</v>
+      </c>
+      <c r="K207">
+        <f>D208</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="208" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
         <v>45076</v>
       </c>
@@ -9705,8 +9850,16 @@
       <c r="F208" s="2">
         <v>4582.6099999999997</v>
       </c>
-    </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I208" s="2">
+        <f>F209</f>
+        <v>4993.8</v>
+      </c>
+      <c r="K208">
+        <f>D209</f>
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="209" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
         <v>45079</v>
       </c>
@@ -9724,17 +9877,34 @@
       </c>
       <c r="F209" s="2">
         <v>4993.8</v>
+      </c>
+      <c r="G209">
+        <f>SUM(F188:F209)</f>
+        <v>223016.36999999997</v>
       </c>
       <c r="H209">
         <f>SUM(D188:D209)</f>
         <v>36950</v>
       </c>
-      <c r="J209">
-        <f>SUM(F188:F209)</f>
-        <v>223016.36999999997</v>
-      </c>
-    </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K209" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="210" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I210" s="2">
+        <f>SUM(I188:I208)</f>
+        <v>223016.37</v>
+      </c>
+      <c r="J210" s="2">
+        <f>G209-I210</f>
+        <v>0</v>
+      </c>
+      <c r="K210" s="2">
+        <f>SUM(K188:K208)</f>
+        <v>36950</v>
+      </c>
+    </row>
+    <row r="211" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
         <v>44988</v>
       </c>
@@ -9754,7 +9924,7 @@
         <v>4716.2</v>
       </c>
     </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
         <v>44988</v>
       </c>
@@ -9782,7 +9952,7 @@
         <v>9418.9</v>
       </c>
     </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
         <v>44986</v>
       </c>
@@ -9802,7 +9972,7 @@
         <v>24860.31</v>
       </c>
     </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
         <v>44986</v>
       </c>
@@ -9822,7 +9992,7 @@
         <v>37088.26</v>
       </c>
     </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
         <v>44988</v>
       </c>
@@ -9842,7 +10012,7 @@
         <v>6514.87</v>
       </c>
     </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
         <v>44988</v>
       </c>
@@ -9862,7 +10032,7 @@
         <v>6512.37</v>
       </c>
     </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
         <v>45019</v>
       </c>
@@ -9882,7 +10052,7 @@
         <v>6339.87</v>
       </c>
     </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A219" s="1">
         <v>45020</v>
       </c>
@@ -9902,7 +10072,7 @@
         <v>6291.02</v>
       </c>
     </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
         <v>45082</v>
       </c>
@@ -9922,7 +10092,7 @@
         <v>62902.76</v>
       </c>
     </row>
-    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
         <v>45085</v>
       </c>
@@ -9950,7 +10120,7 @@
         <v>225033.06</v>
       </c>
     </row>
-    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A223" s="1">
         <v>44988</v>
       </c>
@@ -9970,7 +10140,7 @@
         <v>9500.7000000000007</v>
       </c>
     </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A224" s="1">
         <v>44988</v>
       </c>
@@ -10544,7 +10714,7 @@
       </c>
       <c r="J257" s="2">
         <f>SUM(J188:J255)</f>
-        <v>894562.57000000007</v>
+        <v>671546.2</v>
       </c>
     </row>
   </sheetData>
@@ -10554,21 +10724,24 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:N87"/>
+  <dimension ref="A1:N91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.85546875" style="8" customWidth="1"/>
     <col min="9" max="9" width="9.140625" style="13"/>
+    <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.140625" style="8"/>
     <col min="13" max="13" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>40</v>
       </c>
       <c r="B1" s="7" t="s">
@@ -10596,7 +10769,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>44926</v>
       </c>
@@ -10631,42 +10804,42 @@
       </c>
       <c r="L2" s="8"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>44953</v>
+        <v>44946</v>
       </c>
       <c r="B3" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
       </c>
       <c r="D3">
-        <v>-1000</v>
+        <v>1000</v>
       </c>
       <c r="E3" s="3">
-        <v>5.5124000000000004</v>
+        <v>5.625</v>
       </c>
       <c r="F3" s="8">
-        <f>IF(B3="Sell",D3*E3,D3*E3)</f>
-        <v>-5512.4000000000005</v>
+        <f t="shared" ref="F3:F39" si="0">IF(B3="Sell",D3*E3,D3*E3)</f>
+        <v>5625</v>
       </c>
       <c r="G3">
         <f>G2+D3</f>
-        <v>50</v>
+        <v>2050</v>
       </c>
       <c r="H3" s="8">
-        <f t="shared" ref="H3:H37" si="0">D3*E3</f>
-        <v>-5512.4000000000005</v>
+        <f t="shared" ref="H3:H39" si="1">D3*E3</f>
+        <v>5625</v>
       </c>
       <c r="I3" s="13">
-        <v>-1000</v>
+        <v>0</v>
       </c>
       <c r="L3" s="8"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>44946</v>
+        <v>44949</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
@@ -10678,92 +10851,103 @@
         <v>1000</v>
       </c>
       <c r="E4" s="3">
-        <v>5.625</v>
+        <v>5.7880000000000003</v>
       </c>
       <c r="F4" s="8">
-        <f t="shared" ref="F4:F37" si="1">IF(B4="Sell",D4*E4,D4*E4)</f>
-        <v>5625</v>
+        <f t="shared" si="0"/>
+        <v>5788</v>
       </c>
       <c r="G4">
-        <f t="shared" ref="G4:G37" si="2">G3+D4</f>
-        <v>1050</v>
+        <f t="shared" ref="G4:G39" si="2">G3+D4</f>
+        <v>3050</v>
       </c>
       <c r="H4" s="8">
-        <f t="shared" si="0"/>
-        <v>5625</v>
-      </c>
-      <c r="I4" s="13">
-        <v>0</v>
-      </c>
-      <c r="L4" s="8"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>44949</v>
-      </c>
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5">
-        <v>1000</v>
-      </c>
-      <c r="E5" s="3">
-        <v>5.7880000000000003</v>
-      </c>
-      <c r="F5" s="8">
         <f t="shared" si="1"/>
         <v>5788</v>
       </c>
+      <c r="I4" s="13">
+        <v>0</v>
+      </c>
+      <c r="L4" s="8"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>44953</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>2000</v>
+      </c>
+      <c r="E5" s="3">
+        <v>5.2393999999999998</v>
+      </c>
+      <c r="F5" s="8">
+        <f t="shared" si="0"/>
+        <v>10478.799999999999</v>
+      </c>
       <c r="G5">
         <f t="shared" si="2"/>
-        <v>2050</v>
+        <v>5050</v>
       </c>
       <c r="H5" s="8">
-        <f t="shared" si="0"/>
-        <v>5788</v>
+        <f t="shared" si="1"/>
+        <v>10478.799999999999</v>
       </c>
       <c r="I5" s="13">
         <v>0</v>
       </c>
       <c r="L5" s="8"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>44953</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
       </c>
       <c r="D6">
-        <v>2000</v>
+        <v>-1000</v>
       </c>
       <c r="E6" s="3">
-        <v>5.2393999999999998</v>
+        <v>5.5124000000000004</v>
       </c>
       <c r="F6" s="8">
-        <f t="shared" si="1"/>
-        <v>10478.799999999999</v>
+        <f>IF(B6="Sell",D6*E6,D6*E6)</f>
+        <v>-5512.4000000000005</v>
       </c>
       <c r="G6">
         <f t="shared" si="2"/>
         <v>4050</v>
       </c>
       <c r="H6" s="8">
-        <f t="shared" si="0"/>
-        <v>10478.799999999999</v>
+        <f>D6*E6</f>
+        <v>-5512.4000000000005</v>
       </c>
       <c r="I6" s="13">
-        <v>0</v>
+        <v>-1000</v>
+      </c>
+      <c r="J6" s="8">
+        <f>H6</f>
+        <v>-5512.4000000000005</v>
+      </c>
+      <c r="K6" s="8">
+        <f>H6</f>
+        <v>-5512.4000000000005</v>
       </c>
       <c r="L6" s="8"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N6">
+        <v>5512.12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>44960</v>
       </c>
@@ -10777,11 +10961,11 @@
         <v>-1000</v>
       </c>
       <c r="E7" s="3">
-        <f>L47</f>
+        <f>L49</f>
         <v>6.68255</v>
       </c>
       <c r="F7" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-6682.55</v>
       </c>
       <c r="G7">
@@ -10789,15 +10973,23 @@
         <v>3050</v>
       </c>
       <c r="H7" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-6682.55</v>
       </c>
       <c r="I7" s="13">
         <v>-1000</v>
       </c>
+      <c r="J7" s="8">
+        <f>J6+H7</f>
+        <v>-12194.95</v>
+      </c>
+      <c r="K7" s="8">
+        <f>H7</f>
+        <v>-6682.55</v>
+      </c>
       <c r="L7" s="8"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>44960</v>
       </c>
@@ -10811,11 +11003,11 @@
         <v>-1000</v>
       </c>
       <c r="E8" s="3">
-        <f>E49</f>
+        <f>E51</f>
         <v>6.2549999999999999</v>
       </c>
       <c r="F8" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-6255</v>
       </c>
       <c r="G8">
@@ -10823,15 +11015,26 @@
         <v>2050</v>
       </c>
       <c r="H8" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-6255</v>
       </c>
       <c r="I8" s="13">
         <v>-1000</v>
       </c>
+      <c r="J8" s="8">
+        <f t="shared" ref="J8:J9" si="3">J7+H8</f>
+        <v>-18449.95</v>
+      </c>
+      <c r="K8" s="8">
+        <f>H8</f>
+        <v>-6255</v>
+      </c>
       <c r="L8" s="8"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N8">
+        <v>6680.29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>44960</v>
       </c>
@@ -10845,11 +11048,11 @@
         <v>-1000</v>
       </c>
       <c r="E9" s="3">
-        <f>E51</f>
+        <f>E53</f>
         <v>6.1901000000000002</v>
       </c>
       <c r="F9" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-6190.1</v>
       </c>
       <c r="G9">
@@ -10857,18 +11060,29 @@
         <v>1050</v>
       </c>
       <c r="H9" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-6190.1</v>
       </c>
       <c r="I9" s="13">
         <v>-1000</v>
+      </c>
+      <c r="J9" s="8">
+        <f>J8+H9</f>
+        <v>-24640.050000000003</v>
+      </c>
+      <c r="K9" s="8">
+        <f>H9</f>
+        <v>-6190.1</v>
       </c>
       <c r="L9" s="8"/>
       <c r="M9" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N9">
+        <v>6254.7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>44967</v>
       </c>
@@ -10885,7 +11099,7 @@
         <v>4.7450000000000001</v>
       </c>
       <c r="F10" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>9490</v>
       </c>
       <c r="G10">
@@ -10893,15 +11107,18 @@
         <v>3050</v>
       </c>
       <c r="H10" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9490</v>
       </c>
       <c r="I10" s="13">
         <v>0</v>
       </c>
       <c r="L10" s="8"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N10">
+        <v>6189.8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>44967</v>
       </c>
@@ -10918,7 +11135,7 @@
         <v>4.78</v>
       </c>
       <c r="F11" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>4780</v>
       </c>
       <c r="G11">
@@ -10926,15 +11143,18 @@
         <v>4050</v>
       </c>
       <c r="H11" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4780</v>
       </c>
       <c r="I11" s="13">
         <v>0</v>
       </c>
       <c r="L11" s="8"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N11">
+        <v>17564.150000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>44970</v>
       </c>
@@ -10951,7 +11171,7 @@
         <v>4.7295999999999996</v>
       </c>
       <c r="F12" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>14188.8</v>
       </c>
       <c r="G12">
@@ -10959,7 +11179,7 @@
         <v>7050</v>
       </c>
       <c r="H12" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14188.8</v>
       </c>
       <c r="I12" s="13">
@@ -10969,8 +11189,11 @@
       <c r="M12" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N12">
+        <v>39688.22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>44970</v>
       </c>
@@ -10987,7 +11210,7 @@
         <v>4.7183000000000002</v>
       </c>
       <c r="F13" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>7077.45</v>
       </c>
       <c r="G13">
@@ -10995,7 +11218,7 @@
         <v>8550</v>
       </c>
       <c r="H13" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7077.45</v>
       </c>
       <c r="I13" s="13">
@@ -11003,7 +11226,7 @@
       </c>
       <c r="L13" s="8"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>44970</v>
       </c>
@@ -11020,7 +11243,7 @@
         <v>4.7167000000000003</v>
       </c>
       <c r="F14" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1415.01</v>
       </c>
       <c r="G14">
@@ -11028,7 +11251,7 @@
         <v>8850</v>
       </c>
       <c r="H14" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1415.01</v>
       </c>
       <c r="I14" s="13">
@@ -11036,7 +11259,7 @@
       </c>
       <c r="L14" s="8"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>44970</v>
       </c>
@@ -11053,7 +11276,7 @@
         <v>4.71</v>
       </c>
       <c r="F15" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>9420</v>
       </c>
       <c r="G15">
@@ -11061,15 +11284,18 @@
         <v>10850</v>
       </c>
       <c r="H15" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9420</v>
       </c>
       <c r="I15" s="13">
         <v>0</v>
       </c>
       <c r="L15" s="8"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N15">
+        <v>42069.43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>44972</v>
       </c>
@@ -11086,7 +11312,7 @@
         <v>4.7801</v>
       </c>
       <c r="F16" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>19120.400000000001</v>
       </c>
       <c r="G16">
@@ -11094,15 +11320,18 @@
         <v>14850</v>
       </c>
       <c r="H16" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>19120.400000000001</v>
       </c>
       <c r="I16" s="13">
         <v>0</v>
       </c>
       <c r="L16" s="8"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N16">
+        <v>19653.3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>44978</v>
       </c>
@@ -11119,7 +11348,7 @@
         <v>5.8550000000000004</v>
       </c>
       <c r="F17" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-17565</v>
       </c>
       <c r="G17">
@@ -11127,15 +11356,23 @@
         <v>11850</v>
       </c>
       <c r="H17" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-17565</v>
       </c>
       <c r="I17" s="13">
         <v>-3000</v>
       </c>
+      <c r="J17" s="8">
+        <f>J9+H17</f>
+        <v>-42205.05</v>
+      </c>
+      <c r="K17" s="8">
+        <f>F17</f>
+        <v>-17565</v>
+      </c>
       <c r="L17" s="8"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>44979</v>
       </c>
@@ -11152,7 +11389,7 @@
         <v>6.6150000000000002</v>
       </c>
       <c r="F18" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-39690</v>
       </c>
       <c r="G18">
@@ -11160,809 +11397,901 @@
         <v>5850</v>
       </c>
       <c r="H18" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-39690</v>
       </c>
       <c r="I18" s="13">
         <v>-6000</v>
       </c>
+      <c r="J18" s="8">
+        <f>J17+H18</f>
+        <v>-81895.05</v>
+      </c>
+      <c r="K18" s="8">
+        <f>H18</f>
+        <v>-39690</v>
+      </c>
       <c r="L18" s="8"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="18">
         <v>44984</v>
       </c>
-      <c r="B19" t="s">
-        <v>0</v>
-      </c>
-      <c r="C19" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19">
-        <v>-5850</v>
-      </c>
-      <c r="E19" s="3">
+      <c r="B19" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="19">
+        <v>-3000</v>
+      </c>
+      <c r="E19" s="20">
         <v>7.8159999999999998</v>
       </c>
-      <c r="F19" s="8">
+      <c r="F19" s="21">
+        <f t="shared" si="0"/>
+        <v>-23448</v>
+      </c>
+      <c r="G19" s="19">
+        <f t="shared" si="2"/>
+        <v>2850</v>
+      </c>
+      <c r="H19" s="21">
         <f t="shared" si="1"/>
-        <v>-45723.6</v>
-      </c>
-      <c r="G19">
+        <v>-23448</v>
+      </c>
+      <c r="I19" s="22">
+        <v>-3000</v>
+      </c>
+      <c r="J19" s="21">
+        <f>J18+H19</f>
+        <v>-105343.05</v>
+      </c>
+      <c r="K19" s="21">
+        <f>H19</f>
+        <v>-23448</v>
+      </c>
+      <c r="L19" s="21">
+        <f>E19*D19</f>
+        <v>-23448</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>44984</v>
+      </c>
+      <c r="B20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20">
+        <v>-1850</v>
+      </c>
+      <c r="E20" s="3">
+        <v>7.585</v>
+      </c>
+      <c r="F20" s="8">
+        <f t="shared" si="0"/>
+        <v>-14032.25</v>
+      </c>
+      <c r="G20">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H19" s="8">
+        <v>1000</v>
+      </c>
+      <c r="H20" s="17">
+        <f t="shared" si="1"/>
+        <v>-14032.25</v>
+      </c>
+      <c r="J20" s="8"/>
+      <c r="L20" s="8"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>44984</v>
+      </c>
+      <c r="B21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21">
+        <v>-1000</v>
+      </c>
+      <c r="E21" s="3">
+        <v>7.8159999999999998</v>
+      </c>
+      <c r="F21" s="8">
         <f t="shared" si="0"/>
-        <v>-45723.6</v>
-      </c>
-      <c r="I19" s="13">
-        <v>-5850</v>
-      </c>
-      <c r="L19" s="8"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
+        <v>-7816</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H21" s="17">
+        <f t="shared" si="1"/>
+        <v>-7816</v>
+      </c>
+      <c r="I21" s="13">
+        <v>-2850</v>
+      </c>
+      <c r="J21" s="8">
+        <f>H20+H21+J19</f>
+        <v>-127191.3</v>
+      </c>
+      <c r="L21" s="8"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
         <v>44988</v>
       </c>
-      <c r="B20" t="s">
-        <v>2</v>
-      </c>
-      <c r="C20" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20">
+      <c r="B22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22">
         <v>5000</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E22" s="3">
         <v>6.5891000000000002</v>
       </c>
-      <c r="F20" s="8">
+      <c r="F22" s="8">
+        <f t="shared" si="0"/>
+        <v>32945.5</v>
+      </c>
+      <c r="G22">
+        <f>G21+D22</f>
+        <v>5000</v>
+      </c>
+      <c r="H22" s="8">
         <f t="shared" si="1"/>
         <v>32945.5</v>
       </c>
-      <c r="G20">
+      <c r="I22" s="13">
+        <v>0</v>
+      </c>
+      <c r="L22" s="8"/>
+      <c r="N22">
+        <v>35126.32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>44988</v>
+      </c>
+      <c r="B23" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23">
+        <v>1000</v>
+      </c>
+      <c r="E23" s="3">
+        <v>6.4850000000000003</v>
+      </c>
+      <c r="F23" s="8">
+        <f t="shared" si="0"/>
+        <v>6485</v>
+      </c>
+      <c r="G23">
         <f t="shared" si="2"/>
-        <v>5000</v>
-      </c>
-      <c r="H20" s="8">
-        <f t="shared" si="0"/>
-        <v>32945.5</v>
-      </c>
-      <c r="I20" s="13">
-        <v>0</v>
-      </c>
-      <c r="L20" s="8"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>44988</v>
-      </c>
-      <c r="B21" t="s">
-        <v>2</v>
-      </c>
-      <c r="C21" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21">
-        <v>1000</v>
-      </c>
-      <c r="E21" s="3">
-        <v>6.4850000000000003</v>
-      </c>
-      <c r="F21" s="8">
+        <v>6000</v>
+      </c>
+      <c r="H23" s="8">
         <f t="shared" si="1"/>
         <v>6485</v>
       </c>
-      <c r="G21">
+      <c r="I23" s="13">
+        <v>0</v>
+      </c>
+      <c r="L23" s="8"/>
+      <c r="N23">
+        <v>9829.6299999999992</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>44988</v>
+      </c>
+      <c r="B24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24">
+        <v>-3000</v>
+      </c>
+      <c r="E24" s="3">
+        <v>6.5513000000000003</v>
+      </c>
+      <c r="F24" s="8">
+        <f t="shared" si="0"/>
+        <v>-19653.900000000001</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="2"/>
+        <v>3000</v>
+      </c>
+      <c r="H24" s="8">
+        <f t="shared" si="1"/>
+        <v>-19653.900000000001</v>
+      </c>
+      <c r="I24" s="13">
+        <v>-3000</v>
+      </c>
+      <c r="J24" s="8">
+        <f>J21+H24</f>
+        <v>-146845.20000000001</v>
+      </c>
+      <c r="K24" s="8">
+        <f>H24</f>
+        <v>-19653.900000000001</v>
+      </c>
+      <c r="L24" s="8"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>44992</v>
+      </c>
+      <c r="B25" t="s">
+        <v>2</v>
+      </c>
+      <c r="C25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25">
+        <v>2900</v>
+      </c>
+      <c r="E25" s="3">
+        <v>6.1490999999999998</v>
+      </c>
+      <c r="F25" s="8">
+        <f t="shared" si="0"/>
+        <v>17832.39</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="2"/>
+        <v>5900</v>
+      </c>
+      <c r="H25" s="8">
+        <f t="shared" si="1"/>
+        <v>17832.39</v>
+      </c>
+      <c r="I25" s="13">
+        <v>0</v>
+      </c>
+      <c r="L25" s="8"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>44992</v>
+      </c>
+      <c r="B26" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26">
+        <v>100</v>
+      </c>
+      <c r="E26" s="3">
+        <v>6.1449999999999996</v>
+      </c>
+      <c r="F26" s="8">
+        <f t="shared" si="0"/>
+        <v>614.5</v>
+      </c>
+      <c r="G26">
         <f t="shared" si="2"/>
         <v>6000</v>
       </c>
-      <c r="H21" s="8">
+      <c r="H26" s="8">
+        <f t="shared" si="1"/>
+        <v>614.5</v>
+      </c>
+      <c r="I26" s="13">
+        <v>0</v>
+      </c>
+      <c r="L26" s="8"/>
+      <c r="N26">
+        <v>24872</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>44993</v>
+      </c>
+      <c r="B27" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27">
+        <v>-6000</v>
+      </c>
+      <c r="E27" s="3">
+        <v>5.72</v>
+      </c>
+      <c r="F27" s="8">
         <f t="shared" si="0"/>
-        <v>6485</v>
-      </c>
-      <c r="I21" s="13">
-        <v>0</v>
-      </c>
-      <c r="L21" s="8"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>44988</v>
-      </c>
-      <c r="B22" t="s">
-        <v>0</v>
-      </c>
-      <c r="C22" t="s">
-        <v>5</v>
-      </c>
-      <c r="D22">
-        <v>-3000</v>
-      </c>
-      <c r="E22" s="3">
-        <v>6.5513000000000003</v>
-      </c>
-      <c r="F22" s="8">
+        <v>-34320</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H27" s="8">
         <f t="shared" si="1"/>
-        <v>-19653.900000000001</v>
-      </c>
-      <c r="G22">
+        <v>-34320</v>
+      </c>
+      <c r="I27" s="13">
+        <v>-6000</v>
+      </c>
+      <c r="J27" s="8">
+        <f>J24+H27</f>
+        <v>-181165.2</v>
+      </c>
+      <c r="L27" s="8"/>
+      <c r="N27">
+        <v>4582.6099999999997</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>45001</v>
+      </c>
+      <c r="B28" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28">
+        <v>1000</v>
+      </c>
+      <c r="E28" s="3">
+        <v>4.2949999999999999</v>
+      </c>
+      <c r="F28" s="8">
+        <f t="shared" si="0"/>
+        <v>4295</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="2"/>
+        <v>1000</v>
+      </c>
+      <c r="H28" s="8">
+        <f t="shared" si="1"/>
+        <v>4295</v>
+      </c>
+      <c r="I28" s="13">
+        <v>0</v>
+      </c>
+      <c r="L28" s="8"/>
+      <c r="N28">
+        <v>4993.8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>45001</v>
+      </c>
+      <c r="B29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29">
+        <v>2000</v>
+      </c>
+      <c r="E29" s="3">
+        <v>4.3074000000000003</v>
+      </c>
+      <c r="F29" s="8">
+        <f t="shared" si="0"/>
+        <v>8614.8000000000011</v>
+      </c>
+      <c r="G29">
         <f t="shared" si="2"/>
         <v>3000</v>
       </c>
-      <c r="H22" s="8">
-        <f t="shared" si="0"/>
-        <v>-19653.900000000001</v>
-      </c>
-      <c r="I22" s="13">
-        <v>-3000</v>
-      </c>
-      <c r="L22" s="8"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <v>44992</v>
-      </c>
-      <c r="B23" t="s">
-        <v>2</v>
-      </c>
-      <c r="C23" t="s">
-        <v>5</v>
-      </c>
-      <c r="D23">
-        <v>2900</v>
-      </c>
-      <c r="E23" s="3">
-        <v>6.1490999999999998</v>
-      </c>
-      <c r="F23" s="8">
-        <f t="shared" si="1"/>
-        <v>17832.39</v>
-      </c>
-      <c r="G23">
-        <f t="shared" si="2"/>
-        <v>5900</v>
-      </c>
-      <c r="H23" s="8">
-        <f t="shared" si="0"/>
-        <v>17832.39</v>
-      </c>
-      <c r="I23" s="13">
-        <v>0</v>
-      </c>
-      <c r="L23" s="8"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>44992</v>
-      </c>
-      <c r="B24" t="s">
-        <v>2</v>
-      </c>
-      <c r="C24" t="s">
-        <v>5</v>
-      </c>
-      <c r="D24">
-        <v>100</v>
-      </c>
-      <c r="E24" s="3">
-        <v>6.1449999999999996</v>
-      </c>
-      <c r="F24" s="8">
-        <f t="shared" si="1"/>
-        <v>614.5</v>
-      </c>
-      <c r="G24">
-        <f t="shared" si="2"/>
-        <v>6000</v>
-      </c>
-      <c r="H24" s="8">
-        <f t="shared" si="0"/>
-        <v>614.5</v>
-      </c>
-      <c r="I24" s="13">
-        <v>0</v>
-      </c>
-      <c r="L24" s="8"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <v>44993</v>
-      </c>
-      <c r="B25" t="s">
-        <v>0</v>
-      </c>
-      <c r="C25" t="s">
-        <v>5</v>
-      </c>
-      <c r="D25">
-        <v>-6000</v>
-      </c>
-      <c r="E25" s="3">
-        <v>5.72</v>
-      </c>
-      <c r="F25" s="8">
-        <f t="shared" si="1"/>
-        <v>-34320</v>
-      </c>
-      <c r="G25">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H25" s="8">
-        <f t="shared" si="0"/>
-        <v>-34320</v>
-      </c>
-      <c r="I25" s="13">
-        <v>-6000</v>
-      </c>
-      <c r="L25" s="8"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
-        <v>45001</v>
-      </c>
-      <c r="B26" t="s">
-        <v>2</v>
-      </c>
-      <c r="C26" t="s">
-        <v>5</v>
-      </c>
-      <c r="D26">
-        <v>1000</v>
-      </c>
-      <c r="E26" s="3">
-        <v>4.2949999999999999</v>
-      </c>
-      <c r="F26" s="8">
-        <f t="shared" si="1"/>
-        <v>4295</v>
-      </c>
-      <c r="G26">
-        <f t="shared" si="2"/>
-        <v>1000</v>
-      </c>
-      <c r="H26" s="8">
-        <f t="shared" si="0"/>
-        <v>4295</v>
-      </c>
-      <c r="I26" s="13">
-        <v>0</v>
-      </c>
-      <c r="L26" s="8"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
-        <v>45001</v>
-      </c>
-      <c r="B27" t="s">
-        <v>2</v>
-      </c>
-      <c r="C27" t="s">
-        <v>5</v>
-      </c>
-      <c r="D27">
-        <v>2000</v>
-      </c>
-      <c r="E27" s="3">
-        <v>4.3074000000000003</v>
-      </c>
-      <c r="F27" s="8">
+      <c r="H29" s="8">
         <f t="shared" si="1"/>
         <v>8614.8000000000011</v>
       </c>
-      <c r="G27">
+      <c r="I29" s="13">
+        <v>0</v>
+      </c>
+      <c r="L29" s="8"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>45002</v>
+      </c>
+      <c r="B30" t="s">
+        <v>2</v>
+      </c>
+      <c r="C30" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30">
+        <v>1000</v>
+      </c>
+      <c r="E30" s="3">
+        <v>4.29</v>
+      </c>
+      <c r="F30" s="8">
+        <f t="shared" si="0"/>
+        <v>4290</v>
+      </c>
+      <c r="G30">
         <f t="shared" si="2"/>
-        <v>3000</v>
-      </c>
-      <c r="H27" s="8">
-        <f t="shared" si="0"/>
-        <v>8614.8000000000011</v>
-      </c>
-      <c r="I27" s="13">
-        <v>0</v>
-      </c>
-      <c r="L27" s="8"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
-        <v>45002</v>
-      </c>
-      <c r="B28" t="s">
-        <v>2</v>
-      </c>
-      <c r="C28" t="s">
-        <v>5</v>
-      </c>
-      <c r="D28">
-        <v>1000</v>
-      </c>
-      <c r="E28" s="3">
-        <v>4.29</v>
-      </c>
-      <c r="F28" s="8">
+        <v>4000</v>
+      </c>
+      <c r="H30" s="8">
         <f t="shared" si="1"/>
         <v>4290</v>
       </c>
-      <c r="G28">
-        <f t="shared" si="2"/>
-        <v>4000</v>
-      </c>
-      <c r="H28" s="8">
-        <f t="shared" si="0"/>
-        <v>4290</v>
-      </c>
-      <c r="I28" s="13">
-        <v>0</v>
-      </c>
-      <c r="L28" s="8"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
+      <c r="I30" s="13">
+        <v>0</v>
+      </c>
+      <c r="L30" s="8"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
         <v>45002</v>
       </c>
-      <c r="B29" t="s">
-        <v>2</v>
-      </c>
-      <c r="C29" t="s">
-        <v>5</v>
-      </c>
-      <c r="D29">
+      <c r="B31" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31">
         <v>1000</v>
       </c>
-      <c r="E29" s="3">
+      <c r="E31" s="3">
         <v>4.2249999999999996</v>
       </c>
-      <c r="F29" s="8">
-        <f t="shared" si="1"/>
-        <v>4225</v>
-      </c>
-      <c r="G29">
-        <f t="shared" si="2"/>
-        <v>5000</v>
-      </c>
-      <c r="H29" s="8">
+      <c r="F31" s="8">
         <f t="shared" si="0"/>
         <v>4225</v>
-      </c>
-      <c r="I29" s="13">
-        <v>0</v>
-      </c>
-      <c r="L29" s="8"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
-        <v>45006</v>
-      </c>
-      <c r="B30" t="s">
-        <v>2</v>
-      </c>
-      <c r="C30" t="s">
-        <v>5</v>
-      </c>
-      <c r="D30">
-        <v>2000</v>
-      </c>
-      <c r="E30" s="3">
-        <v>4.42</v>
-      </c>
-      <c r="F30" s="8">
-        <f t="shared" si="1"/>
-        <v>8840</v>
-      </c>
-      <c r="G30">
-        <f t="shared" si="2"/>
-        <v>7000</v>
-      </c>
-      <c r="H30" s="8">
-        <f t="shared" si="0"/>
-        <v>8840</v>
-      </c>
-      <c r="I30" s="13">
-        <v>0</v>
-      </c>
-      <c r="L30" s="8"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
-        <v>45022</v>
-      </c>
-      <c r="B31" t="s">
-        <v>0</v>
-      </c>
-      <c r="C31" t="s">
-        <v>5</v>
-      </c>
-      <c r="D31">
-        <v>-2000</v>
-      </c>
-      <c r="E31" s="3">
-        <v>4.915</v>
-      </c>
-      <c r="F31" s="8">
-        <f t="shared" si="1"/>
-        <v>-9830</v>
       </c>
       <c r="G31">
         <f t="shared" si="2"/>
         <v>5000</v>
       </c>
       <c r="H31" s="8">
+        <f t="shared" si="1"/>
+        <v>4225</v>
+      </c>
+      <c r="I31" s="13">
+        <v>0</v>
+      </c>
+      <c r="L31" s="8"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>45006</v>
+      </c>
+      <c r="B32" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32">
+        <v>2000</v>
+      </c>
+      <c r="E32" s="3">
+        <v>4.42</v>
+      </c>
+      <c r="F32" s="8">
+        <f t="shared" si="0"/>
+        <v>8840</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="2"/>
+        <v>7000</v>
+      </c>
+      <c r="H32" s="8">
+        <f t="shared" si="1"/>
+        <v>8840</v>
+      </c>
+      <c r="I32" s="13">
+        <v>0</v>
+      </c>
+      <c r="L32" s="8"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>45022</v>
+      </c>
+      <c r="B33" t="s">
+        <v>0</v>
+      </c>
+      <c r="C33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33">
+        <v>-2000</v>
+      </c>
+      <c r="E33" s="3">
+        <v>4.915</v>
+      </c>
+      <c r="F33" s="8">
         <f t="shared" si="0"/>
         <v>-9830</v>
       </c>
-      <c r="I31" s="13">
+      <c r="G33">
+        <f t="shared" si="2"/>
+        <v>5000</v>
+      </c>
+      <c r="H33" s="8">
+        <f t="shared" si="1"/>
+        <v>-9830</v>
+      </c>
+      <c r="I33" s="13">
         <v>-2000</v>
       </c>
-      <c r="L31" s="8"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
+      <c r="J33" s="8">
+        <f>J27+H33</f>
+        <v>-190995.20000000001</v>
+      </c>
+      <c r="L33" s="8"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
         <v>45036</v>
       </c>
-      <c r="B32" t="s">
-        <v>0</v>
-      </c>
-      <c r="C32" t="s">
-        <v>5</v>
-      </c>
-      <c r="D32">
+      <c r="B34" t="s">
+        <v>0</v>
+      </c>
+      <c r="C34" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34">
         <v>-5000</v>
       </c>
-      <c r="E32" s="3">
+      <c r="E34" s="3">
         <v>4.9450000000000003</v>
       </c>
-      <c r="F32" s="8">
+      <c r="F34" s="8">
+        <f t="shared" si="0"/>
+        <v>-24725</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H34" s="8">
         <f t="shared" si="1"/>
         <v>-24725</v>
       </c>
-      <c r="G32">
+      <c r="I34" s="13">
+        <v>-5000</v>
+      </c>
+      <c r="J34" s="8">
+        <f>J33+H34</f>
+        <v>-215720.2</v>
+      </c>
+      <c r="L34" s="8"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>45037</v>
+      </c>
+      <c r="B35" t="s">
+        <v>2</v>
+      </c>
+      <c r="C35" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35">
+        <v>400</v>
+      </c>
+      <c r="E35" s="3">
+        <v>5.01</v>
+      </c>
+      <c r="F35" s="8">
+        <f t="shared" si="0"/>
+        <v>2004</v>
+      </c>
+      <c r="G35">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H32" s="8">
-        <f t="shared" si="0"/>
-        <v>-24725</v>
-      </c>
-      <c r="I32" s="13">
-        <v>-5000</v>
-      </c>
-      <c r="L32" s="8"/>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
-        <v>45037</v>
-      </c>
-      <c r="B33" t="s">
-        <v>2</v>
-      </c>
-      <c r="C33" t="s">
-        <v>5</v>
-      </c>
-      <c r="D33">
         <v>400</v>
       </c>
-      <c r="E33" s="3">
-        <v>5.01</v>
-      </c>
-      <c r="F33" s="8">
+      <c r="H35" s="8">
         <f t="shared" si="1"/>
         <v>2004</v>
       </c>
-      <c r="G33">
-        <f t="shared" si="2"/>
-        <v>400</v>
-      </c>
-      <c r="H33" s="8">
-        <f t="shared" si="0"/>
-        <v>2004</v>
-      </c>
-      <c r="I33" s="13">
-        <v>0</v>
-      </c>
-      <c r="L33" s="8"/>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
+      <c r="I35" s="13">
+        <v>0</v>
+      </c>
+      <c r="L35" s="8"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
         <v>45043</v>
       </c>
-      <c r="B34" t="s">
-        <v>2</v>
-      </c>
-      <c r="C34" t="s">
-        <v>5</v>
-      </c>
-      <c r="D34">
+      <c r="B36" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36">
         <v>700</v>
       </c>
-      <c r="E34" s="3">
+      <c r="E36" s="3">
         <v>5.4450000000000003</v>
       </c>
-      <c r="F34" s="8">
-        <f t="shared" si="1"/>
-        <v>3811.5</v>
-      </c>
-      <c r="G34">
-        <f t="shared" si="2"/>
-        <v>1100</v>
-      </c>
-      <c r="H34" s="8">
+      <c r="F36" s="8">
         <f t="shared" si="0"/>
         <v>3811.5</v>
-      </c>
-      <c r="I34" s="13">
-        <v>0</v>
-      </c>
-      <c r="L34" s="8"/>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
-        <v>45063</v>
-      </c>
-      <c r="B35" t="s">
-        <v>2</v>
-      </c>
-      <c r="C35" t="s">
-        <v>5</v>
-      </c>
-      <c r="D35">
-        <v>1000</v>
-      </c>
-      <c r="E35" s="3">
-        <v>5.0090000000000003</v>
-      </c>
-      <c r="F35" s="8">
-        <f t="shared" si="1"/>
-        <v>5009</v>
-      </c>
-      <c r="G35">
-        <f t="shared" si="2"/>
-        <v>2100</v>
-      </c>
-      <c r="H35" s="8">
-        <f t="shared" si="0"/>
-        <v>5009</v>
-      </c>
-      <c r="I35" s="13">
-        <v>0</v>
-      </c>
-      <c r="L35" s="8"/>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
-        <v>45076</v>
-      </c>
-      <c r="B36" t="s">
-        <v>0</v>
-      </c>
-      <c r="C36" t="s">
-        <v>5</v>
-      </c>
-      <c r="D36">
-        <v>-1000</v>
-      </c>
-      <c r="E36" s="3">
-        <v>4.5827999999999998</v>
-      </c>
-      <c r="F36" s="8">
-        <f t="shared" si="1"/>
-        <v>-4582.8</v>
       </c>
       <c r="G36">
         <f t="shared" si="2"/>
         <v>1100</v>
       </c>
       <c r="H36" s="8">
+        <f t="shared" si="1"/>
+        <v>3811.5</v>
+      </c>
+      <c r="I36" s="13">
+        <v>0</v>
+      </c>
+      <c r="L36" s="8"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>45063</v>
+      </c>
+      <c r="B37" t="s">
+        <v>2</v>
+      </c>
+      <c r="C37" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37">
+        <v>1000</v>
+      </c>
+      <c r="E37" s="3">
+        <v>5.0090000000000003</v>
+      </c>
+      <c r="F37" s="8">
+        <f t="shared" si="0"/>
+        <v>5009</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="2"/>
+        <v>2100</v>
+      </c>
+      <c r="H37" s="8">
+        <f t="shared" si="1"/>
+        <v>5009</v>
+      </c>
+      <c r="I37" s="13">
+        <v>0</v>
+      </c>
+      <c r="L37" s="8"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>45076</v>
+      </c>
+      <c r="B38" t="s">
+        <v>0</v>
+      </c>
+      <c r="C38" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38">
+        <v>-1000</v>
+      </c>
+      <c r="E38" s="3">
+        <v>4.5827999999999998</v>
+      </c>
+      <c r="F38" s="8">
         <f t="shared" si="0"/>
         <v>-4582.8</v>
       </c>
-      <c r="I36" s="13">
+      <c r="G38">
+        <f t="shared" si="2"/>
+        <v>1100</v>
+      </c>
+      <c r="H38" s="8">
+        <f t="shared" si="1"/>
+        <v>-4582.8</v>
+      </c>
+      <c r="I38" s="13">
         <v>-1000</v>
       </c>
-      <c r="L36" s="8"/>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
+      <c r="J38" s="8">
+        <f>J34+H38</f>
+        <v>-220303</v>
+      </c>
+      <c r="L38" s="8"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
         <v>45079</v>
       </c>
-      <c r="B37" t="s">
-        <v>0</v>
-      </c>
-      <c r="C37" t="s">
-        <v>5</v>
-      </c>
-      <c r="D37">
+      <c r="B39" t="s">
+        <v>0</v>
+      </c>
+      <c r="C39" t="s">
+        <v>5</v>
+      </c>
+      <c r="D39">
         <v>-1100</v>
       </c>
-      <c r="E37" s="3">
+      <c r="E39" s="3">
         <v>4.54</v>
       </c>
-      <c r="F37" s="8">
+      <c r="F39" s="8">
+        <f t="shared" si="0"/>
+        <v>-4994</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H39" s="8">
         <f t="shared" si="1"/>
         <v>-4994</v>
       </c>
-      <c r="G37">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H37" s="8">
-        <f t="shared" si="0"/>
-        <v>-4994</v>
-      </c>
-      <c r="I37" s="13">
+      <c r="I39" s="13">
         <v>-1100</v>
       </c>
-      <c r="L37" s="8"/>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A38" s="1"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="8">
-        <f>SUM(F2:F37)</f>
-        <v>-35100.699999999997</v>
-      </c>
-      <c r="H38" s="8">
-        <f>SUM(H2:H37)</f>
-        <v>-35100.699999999997</v>
-      </c>
-      <c r="I38" s="13">
-        <f>SUM(I2:I37)</f>
+      <c r="J39" s="8">
+        <f>J38+H39</f>
+        <v>-225297</v>
+      </c>
+      <c r="L39" s="8"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E40" s="3"/>
+      <c r="F40" s="8">
+        <f>SUM(F2:F39)</f>
+        <v>-34673.349999999991</v>
+      </c>
+      <c r="H40" s="8">
+        <f>SUM(H2:H39)</f>
+        <v>-34673.349999999991</v>
+      </c>
+      <c r="I40" s="13">
+        <f>SUM(I2:I39)</f>
         <v>-36950</v>
       </c>
-      <c r="L38" s="8"/>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
+      <c r="J40" s="13">
+        <f>J39</f>
+        <v>-225297</v>
+      </c>
+      <c r="K40" s="8">
+        <v>35100.699999999997</v>
+      </c>
+      <c r="L40" s="8"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D39">
-        <f>SUM(D2:D37)</f>
-        <v>0</v>
-      </c>
-      <c r="E39" s="8" t="s">
+      <c r="D41">
+        <f>SUM(D2:D39)</f>
+        <v>0</v>
+      </c>
+      <c r="E41" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="F39" s="8" t="s">
+      <c r="F41" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G39" s="7">
-        <f>G37</f>
-        <v>0</v>
-      </c>
-      <c r="H39" s="7"/>
-      <c r="I39" s="14"/>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
-      <c r="E40" s="8"/>
-      <c r="G40" s="7"/>
-      <c r="H40" s="7"/>
-      <c r="I40" s="14"/>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+      <c r="G41" s="7">
+        <f>G39</f>
+        <v>0</v>
+      </c>
+      <c r="H41" s="7"/>
+      <c r="I41" s="14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E42" s="8"/>
+      <c r="G42" s="7"/>
+      <c r="H42" s="7"/>
+      <c r="I42" s="14"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D41">
-        <f>SUM(D3:D37)</f>
+      <c r="D43">
+        <f>SUM(D3:D39)</f>
         <v>-1050</v>
       </c>
-      <c r="E41" s="8"/>
-      <c r="G41" s="7"/>
-      <c r="H41" s="7"/>
-      <c r="I41" s="14"/>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
-      <c r="E42" s="3"/>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A43" s="1"/>
-      <c r="D43" t="s">
+      <c r="E43" s="8"/>
+      <c r="G43" s="7"/>
+      <c r="H43" s="7"/>
+      <c r="I43" s="14"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E44" s="3"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D45" t="s">
         <v>22</v>
       </c>
-      <c r="E43" s="3"/>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A44" s="1">
+      <c r="E45" s="3"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
         <v>44953</v>
       </c>
-      <c r="B44" t="s">
-        <v>0</v>
-      </c>
-      <c r="C44" t="s">
-        <v>5</v>
-      </c>
-      <c r="D44">
+      <c r="B46" t="s">
+        <v>0</v>
+      </c>
+      <c r="C46" t="s">
+        <v>5</v>
+      </c>
+      <c r="D46">
         <v>1000</v>
       </c>
-      <c r="E44" s="3">
+      <c r="E46" s="3">
         <v>5.5124000000000004</v>
       </c>
-      <c r="F44" s="8">
+      <c r="F46" s="8">
         <v>5512.12</v>
       </c>
-      <c r="G44">
-        <f>D44</f>
+      <c r="G46">
+        <f>D46</f>
         <v>1000</v>
       </c>
-      <c r="H44">
-        <f>G44</f>
+      <c r="H46">
+        <f>G46</f>
         <v>1000</v>
       </c>
-      <c r="I44" s="13">
-        <f>G44*-1</f>
+      <c r="I46" s="13">
+        <f>G46*-1</f>
         <v>-1000</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A45" s="1"/>
-      <c r="E45" s="3"/>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A46" s="1">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E47" s="3"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
         <v>44960</v>
       </c>
-      <c r="B46" t="s">
-        <v>0</v>
-      </c>
-      <c r="C46" t="s">
-        <v>5</v>
-      </c>
-      <c r="D46">
+      <c r="B48" t="s">
+        <v>0</v>
+      </c>
+      <c r="C48" t="s">
+        <v>5</v>
+      </c>
+      <c r="D48">
         <v>900</v>
       </c>
-      <c r="E46" s="3">
+      <c r="E48" s="3">
         <v>6.6801000000000004</v>
       </c>
-      <c r="F46" s="8">
+      <c r="F48" s="8">
         <v>6011.82</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A47" s="1">
-        <v>44960</v>
-      </c>
-      <c r="B47" t="s">
-        <v>0</v>
-      </c>
-      <c r="C47" t="s">
-        <v>5</v>
-      </c>
-      <c r="D47">
-        <v>100</v>
-      </c>
-      <c r="E47" s="3">
-        <v>6.6849999999999996</v>
-      </c>
-      <c r="F47" s="8">
-        <v>668.47</v>
-      </c>
-      <c r="G47">
-        <v>1000</v>
-      </c>
-      <c r="H47">
-        <f>G47</f>
-        <v>1000</v>
-      </c>
-      <c r="I47" s="13">
-        <f>G47*-1</f>
-        <v>-1000</v>
-      </c>
-      <c r="L47" s="3">
-        <f>SUM(E46:E47)/2</f>
-        <v>6.68255</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A48" s="1"/>
-      <c r="E48" s="3"/>
-      <c r="N48" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>44960</v>
       </c>
@@ -11973,36 +12302,38 @@
         <v>5</v>
       </c>
       <c r="D49">
+        <v>100</v>
+      </c>
+      <c r="E49" s="3">
+        <v>6.6849999999999996</v>
+      </c>
+      <c r="F49" s="8">
+        <v>668.47</v>
+      </c>
+      <c r="G49">
+        <f>D48+D49</f>
         <v>1000</v>
       </c>
-      <c r="E49" s="3">
-        <v>6.2549999999999999</v>
-      </c>
-      <c r="F49" s="8">
-        <v>6254.7</v>
-      </c>
-      <c r="G49">
-        <f>D49</f>
-        <v>1000</v>
-      </c>
       <c r="H49">
-        <f>G49</f>
-        <v>1000</v>
+        <f>H46+G49</f>
+        <v>2000</v>
       </c>
       <c r="I49" s="13">
         <f>G49*-1</f>
         <v>-1000</v>
       </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A50" s="1"/>
+      <c r="L49" s="3">
+        <f>SUM(E48:E49)/2</f>
+        <v>6.68255</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E50" s="3"/>
-      <c r="L50" s="8">
-        <f>F46+F47+F49+F51</f>
-        <v>19124.79</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N50" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>44960</v>
       </c>
@@ -12016,33 +12347,34 @@
         <v>1000</v>
       </c>
       <c r="E51" s="3">
-        <v>6.1901000000000002</v>
+        <v>6.2549999999999999</v>
       </c>
       <c r="F51" s="8">
-        <v>6189.8</v>
+        <v>6254.7</v>
       </c>
       <c r="G51">
+        <f>D51</f>
         <v>1000</v>
       </c>
       <c r="H51">
-        <f>G51</f>
-        <v>1000</v>
+        <f>H49+G51</f>
+        <v>3000</v>
       </c>
       <c r="I51" s="13">
         <f>G51*-1</f>
         <v>-1000</v>
       </c>
-      <c r="L51" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A52" s="1"/>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E52" s="3"/>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L52" s="8">
+        <f>F48+F49+F51+F53</f>
+        <v>19124.79</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>44978</v>
+        <v>44960</v>
       </c>
       <c r="B53" t="s">
         <v>0</v>
@@ -12051,17 +12383,16 @@
         <v>5</v>
       </c>
       <c r="D53">
-        <v>3000</v>
+        <v>1000</v>
       </c>
       <c r="E53" s="3">
-        <v>5.8550000000000004</v>
+        <v>6.1901000000000002</v>
       </c>
       <c r="F53" s="8">
-        <v>17564.150000000001</v>
+        <v>6189.8</v>
       </c>
       <c r="G53">
-        <f>D53</f>
-        <v>3000</v>
+        <v>1000</v>
       </c>
       <c r="H53">
         <f>H51+G53</f>
@@ -12069,16 +12400,18 @@
       </c>
       <c r="I53" s="13">
         <f>G53*-1</f>
-        <v>-3000</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A54" s="1"/>
+        <v>-1000</v>
+      </c>
+      <c r="L53" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E54" s="3"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
-        <v>44979</v>
+        <v>44978</v>
       </c>
       <c r="B55" t="s">
         <v>0</v>
@@ -12087,72 +12420,66 @@
         <v>5</v>
       </c>
       <c r="D55">
-        <v>6000</v>
+        <v>3000</v>
       </c>
       <c r="E55" s="3">
-        <v>6.6150000000000002</v>
+        <v>5.8550000000000004</v>
       </c>
       <c r="F55" s="8">
-        <v>39688.22</v>
+        <v>17564.150000000001</v>
       </c>
       <c r="G55">
         <f>D55</f>
-        <v>6000</v>
+        <v>3000</v>
       </c>
       <c r="H55">
         <f>H53+G55</f>
-        <v>10000</v>
+        <v>7000</v>
       </c>
       <c r="I55" s="13">
         <f>G55*-1</f>
+        <v>-3000</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E56" s="3"/>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>44979</v>
+      </c>
+      <c r="B57" t="s">
+        <v>0</v>
+      </c>
+      <c r="C57" t="s">
+        <v>5</v>
+      </c>
+      <c r="D57">
+        <v>6000</v>
+      </c>
+      <c r="E57" s="3">
+        <v>6.6150000000000002</v>
+      </c>
+      <c r="F57" s="8">
+        <v>39688.22</v>
+      </c>
+      <c r="G57">
+        <f>D57</f>
+        <v>6000</v>
+      </c>
+      <c r="H57">
+        <f>H55+G57</f>
+        <v>13000</v>
+      </c>
+      <c r="I57" s="13">
+        <f>G57*-1</f>
         <v>-6000</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A56" s="1"/>
-      <c r="E56" s="3"/>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A57" s="1">
-        <v>44984</v>
-      </c>
-      <c r="B57" t="s">
-        <v>0</v>
-      </c>
-      <c r="C57" t="s">
-        <v>5</v>
-      </c>
-      <c r="D57">
-        <v>3000</v>
-      </c>
-      <c r="E57" s="3">
-        <v>6.7408000000000001</v>
-      </c>
-      <c r="F57" s="8">
-        <v>20221.79</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A58" s="1">
-        <v>44984</v>
-      </c>
-      <c r="B58" t="s">
-        <v>0</v>
-      </c>
-      <c r="C58" t="s">
-        <v>5</v>
-      </c>
-      <c r="D58">
-        <v>1850</v>
-      </c>
-      <c r="E58" s="3">
-        <v>7.585</v>
-      </c>
-      <c r="F58" s="8">
-        <v>14031.86</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E58" s="3"/>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>44984</v>
       </c>
@@ -12163,90 +12490,100 @@
         <v>5</v>
       </c>
       <c r="D59">
-        <v>1000</v>
+        <v>3000</v>
       </c>
       <c r="E59" s="3">
-        <v>7.8159999999999998</v>
+        <v>6.7408000000000001</v>
       </c>
       <c r="F59" s="8">
-        <v>7815.78</v>
+        <v>20221.79</v>
       </c>
       <c r="G59">
-        <f>SUM(D57:D59)</f>
-        <v>5850</v>
+        <f>D59</f>
+        <v>3000</v>
       </c>
       <c r="H59">
-        <f>H55+G59</f>
-        <v>15850</v>
+        <f>H57+G59</f>
+        <v>16000</v>
       </c>
       <c r="I59" s="13">
         <f>G59*-1</f>
-        <v>-5850</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A60" s="1"/>
+        <v>-3000</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E60" s="3"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
+        <v>44984</v>
+      </c>
+      <c r="B61" t="s">
+        <v>0</v>
+      </c>
+      <c r="C61" t="s">
+        <v>5</v>
+      </c>
+      <c r="D61">
+        <v>1850</v>
+      </c>
+      <c r="E61" s="3">
+        <v>7.585</v>
+      </c>
+      <c r="F61" s="8">
+        <v>14031.86</v>
+      </c>
+      <c r="G61" t="s">
+        <v>22</v>
+      </c>
+      <c r="H61" t="s">
+        <v>22</v>
+      </c>
+      <c r="I61" s="13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <v>44984</v>
+      </c>
+      <c r="B62" t="s">
+        <v>0</v>
+      </c>
+      <c r="C62" t="s">
+        <v>5</v>
+      </c>
+      <c r="D62">
+        <v>1000</v>
+      </c>
+      <c r="E62" s="3">
+        <v>7.8159999999999998</v>
+      </c>
+      <c r="F62" s="8">
+        <v>7815.78</v>
+      </c>
+      <c r="G62">
+        <f>D61+D62</f>
+        <v>2850</v>
+      </c>
+      <c r="H62">
+        <f>H59+G62</f>
+        <v>18850</v>
+      </c>
+      <c r="I62" s="13">
+        <f>G62*-1</f>
+        <v>-2850</v>
+      </c>
+      <c r="K62" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E63" s="3"/>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
         <v>44988</v>
-      </c>
-      <c r="B61" t="s">
-        <v>0</v>
-      </c>
-      <c r="C61" t="s">
-        <v>5</v>
-      </c>
-      <c r="D61">
-        <v>3000</v>
-      </c>
-      <c r="E61" s="3">
-        <v>6.5513000000000003</v>
-      </c>
-      <c r="F61" s="8">
-        <v>19653.3</v>
-      </c>
-      <c r="G61">
-        <f>D61</f>
-        <v>3000</v>
-      </c>
-      <c r="H61">
-        <f>H59+G61</f>
-        <v>18850</v>
-      </c>
-      <c r="I61" s="13">
-        <f>G61*-1</f>
-        <v>-3000</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A62" s="1"/>
-      <c r="E62" s="3"/>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A63" s="1">
-        <v>44993</v>
-      </c>
-      <c r="B63" t="s">
-        <v>0</v>
-      </c>
-      <c r="C63" t="s">
-        <v>5</v>
-      </c>
-      <c r="D63">
-        <v>500</v>
-      </c>
-      <c r="E63" s="3">
-        <v>5.8449999999999998</v>
-      </c>
-      <c r="F63" s="8">
-        <v>2922.4</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A64" s="1">
-        <v>44993</v>
       </c>
       <c r="B64" t="s">
         <v>0</v>
@@ -12258,31 +12595,26 @@
         <v>3000</v>
       </c>
       <c r="E64" s="3">
-        <v>5.9450000000000003</v>
+        <v>6.5513000000000003</v>
       </c>
       <c r="F64" s="8">
-        <v>17834.41</v>
+        <v>19653.3</v>
+      </c>
+      <c r="G64">
+        <f>D64</f>
+        <v>3000</v>
+      </c>
+      <c r="H64">
+        <f>H62+G64</f>
+        <v>21850</v>
+      </c>
+      <c r="I64" s="13">
+        <f>G64*-1</f>
+        <v>-3000</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A65" s="1">
-        <v>44993</v>
-      </c>
-      <c r="B65" t="s">
-        <v>0</v>
-      </c>
-      <c r="C65" t="s">
-        <v>5</v>
-      </c>
-      <c r="D65">
-        <v>2000</v>
-      </c>
-      <c r="E65" s="3">
-        <v>5.7549999999999999</v>
-      </c>
-      <c r="F65" s="8">
-        <v>11509.61</v>
-      </c>
+      <c r="E65" s="3"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
@@ -12298,67 +12630,70 @@
         <v>500</v>
       </c>
       <c r="E66" s="3">
-        <v>5.72</v>
+        <v>5.8449999999999998</v>
       </c>
       <c r="F66" s="8">
-        <v>2859.9</v>
-      </c>
-      <c r="G66">
-        <f>SUM(D63:D66)</f>
-        <v>6000</v>
-      </c>
-      <c r="H66">
-        <f>H61+G66</f>
-        <v>24850</v>
-      </c>
-      <c r="I66" s="13">
-        <f>G66*-1</f>
-        <v>-6000</v>
+        <v>2922.4</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A67" s="1"/>
-      <c r="E67" s="3"/>
+      <c r="A67" s="1">
+        <v>44993</v>
+      </c>
+      <c r="B67" t="s">
+        <v>0</v>
+      </c>
+      <c r="C67" t="s">
+        <v>5</v>
+      </c>
+      <c r="D67">
+        <v>3000</v>
+      </c>
+      <c r="E67" s="3">
+        <v>5.9450000000000003</v>
+      </c>
+      <c r="F67" s="8">
+        <v>17834.41</v>
+      </c>
+      <c r="G67">
+        <f>SUM(D66:D67)</f>
+        <v>3500</v>
+      </c>
+      <c r="H67">
+        <f>H64+G67</f>
+        <v>25350</v>
+      </c>
+      <c r="I67" s="13">
+        <f>G67*-1</f>
+        <v>-3500</v>
+      </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A68" s="1">
-        <v>45022</v>
-      </c>
-      <c r="B68" t="s">
-        <v>0</v>
-      </c>
-      <c r="C68" t="s">
-        <v>5</v>
-      </c>
-      <c r="D68">
+      <c r="E68" s="3"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
+        <v>44993</v>
+      </c>
+      <c r="B69" t="s">
+        <v>0</v>
+      </c>
+      <c r="C69" t="s">
+        <v>5</v>
+      </c>
+      <c r="D69">
         <v>2000</v>
       </c>
-      <c r="E68" s="3">
-        <v>4.915</v>
-      </c>
-      <c r="F68" s="8">
-        <v>9829.6299999999992</v>
-      </c>
-      <c r="G68">
-        <f>D68</f>
-        <v>2000</v>
-      </c>
-      <c r="H68">
-        <f>H66+G68</f>
-        <v>26850</v>
-      </c>
-      <c r="I68" s="13">
-        <f>G68*-1</f>
-        <v>-2000</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A69" s="1"/>
-      <c r="E69" s="3"/>
+      <c r="E69" s="3">
+        <v>5.7549999999999999</v>
+      </c>
+      <c r="F69" s="8">
+        <v>11509.61</v>
+      </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
-        <v>45036</v>
+        <v>44993</v>
       </c>
       <c r="B70" t="s">
         <v>0</v>
@@ -12367,94 +12702,88 @@
         <v>5</v>
       </c>
       <c r="D70">
-        <v>3000</v>
+        <v>500</v>
       </c>
       <c r="E70" s="3">
-        <v>4.9893999999999998</v>
+        <v>5.72</v>
       </c>
       <c r="F70" s="8">
-        <v>14967.64</v>
+        <v>2859.9</v>
+      </c>
+      <c r="G70">
+        <f>D69+D70</f>
+        <v>2500</v>
+      </c>
+      <c r="H70">
+        <f>H67+G70</f>
+        <v>27850</v>
+      </c>
+      <c r="I70" s="13">
+        <f>G70*-1</f>
+        <v>-2500</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A71" s="1">
-        <v>45036</v>
-      </c>
-      <c r="B71" t="s">
-        <v>0</v>
-      </c>
-      <c r="C71" t="s">
-        <v>5</v>
-      </c>
-      <c r="D71">
-        <v>190</v>
-      </c>
-      <c r="E71" s="3">
-        <v>4.97</v>
-      </c>
-      <c r="F71" s="8">
-        <v>944.26</v>
-      </c>
+      <c r="E71" s="3"/>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
+        <v>45022</v>
+      </c>
+      <c r="B72" t="s">
+        <v>0</v>
+      </c>
+      <c r="C72" t="s">
+        <v>5</v>
+      </c>
+      <c r="D72">
+        <v>2000</v>
+      </c>
+      <c r="E72" s="3">
+        <v>4.915</v>
+      </c>
+      <c r="F72" s="8">
+        <v>9829.6299999999992</v>
+      </c>
+      <c r="G72">
+        <f>D72</f>
+        <v>2000</v>
+      </c>
+      <c r="H72">
+        <f>H70+G72</f>
+        <v>29850</v>
+      </c>
+      <c r="I72" s="13">
+        <f>G72*-1</f>
+        <v>-2000</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E73" s="3"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74" s="1">
         <v>45036</v>
       </c>
-      <c r="B72" t="s">
-        <v>0</v>
-      </c>
-      <c r="C72" t="s">
-        <v>5</v>
-      </c>
-      <c r="D72">
-        <v>1000</v>
-      </c>
-      <c r="E72" s="3">
-        <v>4.9550000000000001</v>
-      </c>
-      <c r="F72" s="8">
-        <v>4954.8100000000004</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A73" s="1">
-        <v>45036</v>
-      </c>
-      <c r="B73" t="s">
-        <v>0</v>
-      </c>
-      <c r="C73" t="s">
-        <v>5</v>
-      </c>
-      <c r="D73">
-        <v>810</v>
-      </c>
-      <c r="E73" s="3">
-        <v>4.9450000000000003</v>
-      </c>
-      <c r="F73" s="8">
-        <v>4005.29</v>
-      </c>
-      <c r="G73">
-        <f>SUM(D70:D73)</f>
-        <v>5000</v>
-      </c>
-      <c r="H73">
-        <f>H68+G73</f>
-        <v>31850</v>
-      </c>
-      <c r="I73" s="13">
-        <f>G73*-1</f>
-        <v>-5000</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A74" s="1"/>
-      <c r="E74" s="3"/>
+      <c r="B74" t="s">
+        <v>0</v>
+      </c>
+      <c r="C74" t="s">
+        <v>5</v>
+      </c>
+      <c r="D74">
+        <v>3000</v>
+      </c>
+      <c r="E74" s="3">
+        <v>4.9893999999999998</v>
+      </c>
+      <c r="F74" s="8">
+        <v>14967.64</v>
+      </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
-        <v>45076</v>
+        <v>45036</v>
       </c>
       <c r="B75" t="s">
         <v>0</v>
@@ -12463,34 +12792,38 @@
         <v>5</v>
       </c>
       <c r="D75">
+        <v>190</v>
+      </c>
+      <c r="E75" s="3">
+        <v>4.97</v>
+      </c>
+      <c r="F75" s="8">
+        <v>944.26</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76" s="1">
+        <v>45036</v>
+      </c>
+      <c r="B76" t="s">
+        <v>0</v>
+      </c>
+      <c r="C76" t="s">
+        <v>5</v>
+      </c>
+      <c r="D76">
         <v>1000</v>
       </c>
-      <c r="E75" s="3">
-        <v>4.5827999999999998</v>
-      </c>
-      <c r="F75" s="8">
-        <v>4582.6099999999997</v>
-      </c>
-      <c r="G75">
-        <f>D75</f>
-        <v>1000</v>
-      </c>
-      <c r="H75">
-        <f>H73+G75</f>
-        <v>32850</v>
-      </c>
-      <c r="I75" s="13">
-        <f>G75*-1</f>
-        <v>-1000</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A76" s="1"/>
-      <c r="E76" s="3"/>
+      <c r="E76" s="3">
+        <v>4.9550000000000001</v>
+      </c>
+      <c r="F76" s="8">
+        <v>4954.8100000000004</v>
+      </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
-        <v>45079</v>
+        <v>45036</v>
       </c>
       <c r="B77" t="s">
         <v>0</v>
@@ -12499,106 +12832,169 @@
         <v>5</v>
       </c>
       <c r="D77">
-        <v>1100</v>
+        <v>810</v>
       </c>
       <c r="E77" s="3">
-        <v>4.54</v>
+        <v>4.9450000000000003</v>
       </c>
       <c r="F77" s="8">
-        <v>4993.8</v>
+        <v>4005.29</v>
       </c>
       <c r="G77">
-        <f>D77</f>
-        <v>1100</v>
+        <f>SUM(D74:D77)</f>
+        <v>5000</v>
       </c>
       <c r="H77">
-        <f>H75+G77</f>
-        <v>33950</v>
+        <f>H72+G77</f>
+        <v>34850</v>
       </c>
       <c r="I77" s="13">
         <f>G77*-1</f>
+        <v>-5000</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E78" s="3"/>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
+        <v>45076</v>
+      </c>
+      <c r="B79" t="s">
+        <v>0</v>
+      </c>
+      <c r="C79" t="s">
+        <v>5</v>
+      </c>
+      <c r="D79">
+        <v>1000</v>
+      </c>
+      <c r="E79" s="3">
+        <v>4.5827999999999998</v>
+      </c>
+      <c r="F79" s="8">
+        <v>4582.6099999999997</v>
+      </c>
+      <c r="G79">
+        <f>D79</f>
+        <v>1000</v>
+      </c>
+      <c r="H79">
+        <f>H77+G79</f>
+        <v>35850</v>
+      </c>
+      <c r="I79" s="13">
+        <f>G79*-1</f>
+        <v>-1000</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E80" s="3"/>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A81" s="1">
+        <v>45079</v>
+      </c>
+      <c r="B81" t="s">
+        <v>0</v>
+      </c>
+      <c r="C81" t="s">
+        <v>5</v>
+      </c>
+      <c r="D81">
+        <v>1100</v>
+      </c>
+      <c r="E81" s="3">
+        <v>4.54</v>
+      </c>
+      <c r="F81" s="8">
+        <v>4993.8</v>
+      </c>
+      <c r="G81">
+        <f>D81</f>
+        <v>1100</v>
+      </c>
+      <c r="H81">
+        <f>H79+G81</f>
+        <v>36950</v>
+      </c>
+      <c r="I81" s="13">
+        <f>G81*-1</f>
         <v>-1100</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D79">
-        <f>SUM(D44:D78)</f>
+      <c r="D83">
+        <f>SUM(D46:D82)</f>
         <v>36950</v>
       </c>
-      <c r="E79" s="8">
-        <f>SUM(E44:E78)/22</f>
-        <v>5.8930863636363648</v>
-      </c>
-      <c r="F79" s="8">
-        <f>SUM(F44:F78)/D79</f>
+      <c r="E83" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F83" s="8">
+        <f>SUM(F46:F82)/D83</f>
         <v>6.0356257104194846</v>
       </c>
-      <c r="G79">
-        <f>SUM(G44:G77)</f>
+      <c r="G83">
+        <f>SUM(G46:G81)</f>
         <v>36950</v>
       </c>
-      <c r="I79">
-        <f>SUM(I44:I77)</f>
+      <c r="I83">
+        <f>SUM(I46:I81)</f>
         <v>-36950</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A80" s="1"/>
-      <c r="E80" s="3"/>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E84" s="3"/>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D81">
-        <f>D79-D39</f>
+      <c r="D85">
+        <f>D83-D41</f>
         <v>36950</v>
       </c>
-      <c r="E81" s="8" t="e">
-        <f t="shared" ref="E81:G81" si="3">E79-E39</f>
+      <c r="E85" t="e">
+        <f>E83-E41</f>
         <v>#VALUE!</v>
       </c>
-      <c r="F81" s="8" t="e">
-        <f t="shared" si="3"/>
+      <c r="F85" s="8" t="e">
+        <f>F8-F41</f>
         <v>#VALUE!</v>
       </c>
-      <c r="G81">
-        <f t="shared" si="3"/>
+      <c r="G85">
+        <f>G83-G41</f>
         <v>36950</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E82" s="3"/>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A83" s="1"/>
-      <c r="E83" s="3"/>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A84" s="1"/>
-      <c r="E84" s="3"/>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A85" s="1"/>
-      <c r="E85" s="3"/>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A86" s="1"/>
       <c r="E86" s="3"/>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A87" s="1"/>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E87" s="3"/>
     </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E88" s="3"/>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E89" s="3"/>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E90" s="3"/>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E91" s="3"/>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A46:F77">
-    <sortCondition ref="A46:A77"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A48:F81">
+    <sortCondition ref="A48:A81"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13360,7 +13756,7 @@
         <v>6680.29</v>
       </c>
       <c r="O19" s="1">
-        <f t="shared" ref="N19:O19" si="4">O18</f>
+        <f t="shared" ref="O19" si="4">O18</f>
         <v>44960</v>
       </c>
       <c r="P19" s="8">

</xml_diff>